<commit_message>
cest pas vrai que je fais faire 33 commit pour chacun de mes tests XD
</commit_message>
<xml_diff>
--- a/TP2/tableau de choix et contraintes utile pour l'eventuel rapport.xlsx
+++ b/TP2/tableau de choix et contraintes utile pour l'eventuel rapport.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="51">
   <si>
     <t>nb vertices</t>
   </si>
@@ -96,6 +96,87 @@
   </si>
   <si>
     <t>0 &lt; e &lt; sum 0 a v-1</t>
+  </si>
+  <si>
+    <t>simple int int</t>
+  </si>
+  <si>
+    <t>simple int double</t>
+  </si>
+  <si>
+    <t>p1</t>
+  </si>
+  <si>
+    <t>p == 0</t>
+  </si>
+  <si>
+    <t>p2</t>
+  </si>
+  <si>
+    <t>0 &lt; p &lt; 1</t>
+  </si>
+  <si>
+    <t>p3</t>
+  </si>
+  <si>
+    <t>p == 1</t>
+  </si>
+  <si>
+    <t>p4</t>
+  </si>
+  <si>
+    <t>p &lt; 0</t>
+  </si>
+  <si>
+    <t>p5</t>
+  </si>
+  <si>
+    <t>p &gt; 1</t>
+  </si>
+  <si>
+    <t>bipartite vVe</t>
+  </si>
+  <si>
+    <t>v &lt; 0</t>
+  </si>
+  <si>
+    <t>e&lt;0</t>
+  </si>
+  <si>
+    <t>V1</t>
+  </si>
+  <si>
+    <t>V &lt; 0</t>
+  </si>
+  <si>
+    <t>ok, gauchevide</t>
+  </si>
+  <si>
+    <t>V2</t>
+  </si>
+  <si>
+    <t>V == 0</t>
+  </si>
+  <si>
+    <t>ok, droitevide</t>
+  </si>
+  <si>
+    <t>V &gt;= 1</t>
+  </si>
+  <si>
+    <t>0 &lt;= e &lt;= v*V</t>
+  </si>
+  <si>
+    <t>e &gt; v*V</t>
+  </si>
+  <si>
+    <t>V3</t>
+  </si>
+  <si>
+    <t>0 &lt;= p &lt;= 1</t>
+  </si>
+  <si>
+    <t>bipartite vVp</t>
   </si>
 </sst>
 </file>
@@ -217,7 +298,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -229,6 +310,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -509,10 +592,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="D4:K21"/>
+  <dimension ref="A4:U24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D9" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+    <sheetView tabSelected="1" topLeftCell="J6" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="W14" sqref="W14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -520,7 +603,7 @@
     <col min="1" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="4:11" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D4" s="1" t="s">
         <v>0</v>
       </c>
@@ -528,7 +611,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="4:11" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D6" s="1" t="s">
         <v>1</v>
       </c>
@@ -536,107 +619,390 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="4:11" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="P10" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>2</v>
+      </c>
       <c r="I11" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="L11" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="K11" s="3" t="s">
+      <c r="N11" s="3" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="12" spans="4:11" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="I12" s="6"/>
-      <c r="K12" s="4"/>
-    </row>
-    <row r="13" spans="4:11" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="H13" s="7" t="s">
+      <c r="Q11" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="S11" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="6"/>
+      <c r="D12" s="4"/>
+      <c r="G12" s="6"/>
+      <c r="I12" s="4"/>
+      <c r="L12" s="6"/>
+      <c r="N12" s="4"/>
+      <c r="Q12" s="6"/>
+      <c r="S12" s="4"/>
+    </row>
+    <row r="13" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="7" t="s">
         <v>12</v>
       </c>
+      <c r="B13" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C13" s="8"/>
+      <c r="D13" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F13" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H13" s="8"/>
       <c r="I13" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="J13" s="8"/>
-      <c r="K13" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="14" spans="4:11" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="H14" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="J13" s="12"/>
+      <c r="K13" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="L13" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="M13" s="8"/>
+      <c r="N13" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="P13" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q13" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="R13" s="8"/>
+      <c r="S13" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="9" t="s">
         <v>13</v>
       </c>
+      <c r="B14" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F14" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="G14" s="4" t="s">
+        <v>3</v>
+      </c>
       <c r="I14" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="K14" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="L14" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="K14" s="4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="15" spans="4:11" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="H15" s="9" t="s">
+      <c r="N14" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="P14" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q14" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="S14" s="4" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="9" t="s">
         <v>14</v>
       </c>
+      <c r="B15" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F15" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="G15" s="4" t="s">
+        <v>17</v>
+      </c>
       <c r="I15" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="K15" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="L15" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="K15" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="16" spans="4:11" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="H16" s="10" t="s">
+      <c r="N15" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="P15" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q15" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="S15" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="I16" s="5" t="s">
+      <c r="B16" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="J16" s="2"/>
-      <c r="K16" s="5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="17" spans="8:11" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="I17" s="4"/>
-    </row>
-    <row r="18" spans="8:11" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="I18" s="4"/>
-      <c r="K18" s="3" t="s">
+      <c r="C16" s="2"/>
+      <c r="D16" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F16" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="G16" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="I16" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="K16" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="L16" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="N16" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="P16" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q16" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="S16" s="12" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:21" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="4"/>
+      <c r="F17" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="G17" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="I17" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="K17" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="L17" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="N17" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="P17" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q17" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="S17" s="12" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:21" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="4"/>
+      <c r="D18" s="3" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="19" spans="8:11" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="H19" s="7" t="s">
+      <c r="K18" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="L18" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="N18" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="P18" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q18" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="S18" s="11" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:21" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="I19" s="3" t="s">
+      <c r="B19" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="J19" s="8"/>
-      <c r="K19" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="20" spans="8:11" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="H20" s="9" t="s">
+      <c r="C19" s="8"/>
+      <c r="D19" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F19" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="G19" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="I19" s="11" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:21" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="I20" s="4" t="s">
+      <c r="B20" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="K20" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="21" spans="8:11" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="H21" s="10" t="s">
+      <c r="D20" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F20" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="G20" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="I20" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="K20" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="L20" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="N20" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="P20" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q20" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="S20" s="12" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="21" spans="1:21" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="I21" s="5" t="s">
+      <c r="B21" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="J21" s="2"/>
-      <c r="K21" s="5" t="s">
-        <v>5</v>
-      </c>
+      <c r="C21" s="2"/>
+      <c r="D21" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="F21" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="G21" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="I21" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="K21" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="L21" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="N21" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="P21" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q21" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="S21" s="12" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:21" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K22" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="L22" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="N22" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="P22" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q22" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="S22" s="12" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:21" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="R24" s="11"/>
+      <c r="S24" s="11"/>
+      <c r="U24" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
ajout dans excel de fonction regular
</commit_message>
<xml_diff>
--- a/TP2/tableau de choix et contraintes utile pour l'eventuel rapport.xlsx
+++ b/TP2/tableau de choix et contraintes utile pour l'eventuel rapport.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="63">
   <si>
     <t>nb vertices</t>
   </si>
@@ -177,6 +177,42 @@
   </si>
   <si>
     <t>bipartite vVp</t>
+  </si>
+  <si>
+    <t>regular</t>
+  </si>
+  <si>
+    <t>propriété</t>
+  </si>
+  <si>
+    <t>v &gt; 0</t>
+  </si>
+  <si>
+    <t>k1</t>
+  </si>
+  <si>
+    <t>contrainte</t>
+  </si>
+  <si>
+    <t>k2</t>
+  </si>
+  <si>
+    <t>k &lt; 0</t>
+  </si>
+  <si>
+    <t>k3</t>
+  </si>
+  <si>
+    <t>k &gt; v-1</t>
+  </si>
+  <si>
+    <t>k4</t>
+  </si>
+  <si>
+    <t>k == 0</t>
+  </si>
+  <si>
+    <t>0 &lt; k &lt; v-1</t>
   </si>
 </sst>
 </file>
@@ -298,7 +334,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -312,6 +348,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -592,10 +633,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A4:U24"/>
+  <dimension ref="A4:X24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J6" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="W14" sqref="W14"/>
+    <sheetView tabSelected="1" topLeftCell="B5" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="V25" sqref="V25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -603,7 +644,7 @@
     <col min="1" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D4" s="1" t="s">
         <v>0</v>
       </c>
@@ -611,7 +652,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D6" s="1" t="s">
         <v>1</v>
       </c>
@@ -619,7 +660,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>24</v>
       </c>
@@ -632,8 +673,11 @@
       <c r="P10" s="1" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="11" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="U10" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="11" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="3" t="s">
         <v>2</v>
       </c>
@@ -658,8 +702,14 @@
       <c r="S11" s="3" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="12" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="V11" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="X11" s="3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="12" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="6"/>
       <c r="D12" s="4"/>
       <c r="G12" s="6"/>
@@ -668,8 +718,10 @@
       <c r="N12" s="4"/>
       <c r="Q12" s="6"/>
       <c r="S12" s="4"/>
-    </row>
-    <row r="13" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="V12" s="4"/>
+      <c r="X12" s="4"/>
+    </row>
+    <row r="13" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>12</v>
       </c>
@@ -690,7 +742,7 @@
       <c r="I13" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="J13" s="12"/>
+      <c r="J13" s="13"/>
       <c r="K13" s="7" t="s">
         <v>12</v>
       </c>
@@ -711,8 +763,18 @@
       <c r="S13" s="3" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="14" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="U13" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="V13" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="W13" s="8"/>
+      <c r="X13" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
         <v>13</v>
       </c>
@@ -749,8 +811,17 @@
       <c r="S14" s="4" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="15" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="U14" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="V14" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="X14" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="9" t="s">
         <v>14</v>
       </c>
@@ -787,8 +858,17 @@
       <c r="S15" s="4" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="16" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="U15" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="V15" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="X15" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="10" t="s">
         <v>11</v>
       </c>
@@ -799,7 +879,7 @@
       <c r="D16" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="F16" s="11" t="s">
+      <c r="F16" s="13" t="s">
         <v>32</v>
       </c>
       <c r="G16" s="12" t="s">
@@ -808,7 +888,7 @@
       <c r="I16" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="K16" s="11" t="s">
+      <c r="K16" s="13" t="s">
         <v>39</v>
       </c>
       <c r="L16" s="12" t="s">
@@ -817,7 +897,7 @@
       <c r="N16" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="P16" s="11" t="s">
+      <c r="P16" s="13" t="s">
         <v>39</v>
       </c>
       <c r="Q16" s="12" t="s">
@@ -826,19 +906,29 @@
       <c r="S16" s="12" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="17" spans="1:21" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="U16" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="V16" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="X16" s="12" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="4"/>
-      <c r="F17" s="11" t="s">
+      <c r="F17" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="G17" s="12" t="s">
+      <c r="G17" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="I17" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="K17" s="11" t="s">
+      <c r="H17" s="2"/>
+      <c r="I17" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="K17" s="13" t="s">
         <v>8</v>
       </c>
       <c r="L17" s="12" t="s">
@@ -847,7 +937,7 @@
       <c r="N17" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="P17" s="11" t="s">
+      <c r="P17" s="13" t="s">
         <v>26</v>
       </c>
       <c r="Q17" s="12" t="s">
@@ -856,32 +946,46 @@
       <c r="S17" s="12" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="18" spans="1:21" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="U17" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="V17" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="W17" s="2"/>
+      <c r="X17" s="15" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="4"/>
       <c r="D18" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="K18" s="11" t="s">
+      <c r="G18" s="4"/>
+      <c r="K18" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="L18" s="11" t="s">
+      <c r="L18" s="15" t="s">
         <v>47</v>
       </c>
-      <c r="N18" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="P18" s="11" t="s">
+      <c r="M18" s="2"/>
+      <c r="N18" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="P18" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="Q18" s="11" t="s">
+      <c r="Q18" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="S18" s="11" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="19" spans="1:21" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="R18" s="2"/>
+      <c r="S18" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="V18" s="4"/>
+    </row>
+    <row r="19" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
         <v>8</v>
       </c>
@@ -892,17 +996,15 @@
       <c r="D19" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="F19" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="G19" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="I19" s="11" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="20" spans="1:21" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G19" s="4"/>
+      <c r="I19" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="L19" s="4"/>
+      <c r="Q19" s="4"/>
+      <c r="V19" s="4"/>
+    </row>
+    <row r="20" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="9" t="s">
         <v>9</v>
       </c>
@@ -912,35 +1014,30 @@
       <c r="D20" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="F20" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="G20" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="I20" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="K20" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="L20" s="12" t="s">
-        <v>43</v>
-      </c>
-      <c r="N20" s="12" t="s">
-        <v>44</v>
-      </c>
-      <c r="P20" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q20" s="12" t="s">
-        <v>43</v>
-      </c>
-      <c r="S20" s="12" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="21" spans="1:21" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F20" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="G20" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="H20" s="8"/>
+      <c r="I20" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="L20" s="4"/>
+      <c r="N20" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q20" s="4"/>
+      <c r="S20" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="V20" s="4"/>
+      <c r="X20" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="21" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="10" t="s">
         <v>10</v>
       </c>
@@ -951,55 +1048,109 @@
       <c r="D21" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="F21" s="11" t="s">
+      <c r="F21" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="G21" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="I21" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="K21" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="L21" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="M21" s="8"/>
+      <c r="N21" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="P21" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q21" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="R21" s="8"/>
+      <c r="S21" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="U21" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="V21" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="W21" s="8"/>
+      <c r="X21" s="17" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F22" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="G21" s="11" t="s">
+      <c r="G22" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="I21" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="K21" s="11" t="s">
+      <c r="H22" s="2"/>
+      <c r="I22" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="K22" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="L21" s="12" t="s">
+      <c r="L22" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="N21" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="P21" s="11" t="s">
+      <c r="N22" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="P22" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="Q21" s="12" t="s">
+      <c r="Q22" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="S21" s="12" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="22" spans="1:21" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K22" s="11" t="s">
+      <c r="S22" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="U22" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="V22" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="W22" s="2"/>
+      <c r="X22" s="15" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K23" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="L22" s="12" t="s">
+      <c r="L23" s="15" t="s">
         <v>46</v>
       </c>
-      <c r="N22" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="P22" s="11" t="s">
+      <c r="M23" s="2"/>
+      <c r="N23" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="P23" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="Q22" s="12" t="s">
+      <c r="Q23" s="15" t="s">
         <v>49</v>
       </c>
-      <c r="S22" s="12" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="24" spans="1:21" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="R23" s="2"/>
+      <c r="S23" s="15" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="R24" s="11"/>
       <c r="S24" s="11"/>
       <c r="U24" s="11"/>

</xml_diff>